<commit_message>
cambios de tipos de datos
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/branch/BranchFormulario.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/branch/BranchFormulario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ReposAxsis\API\Service.Catalog\wwwroot\layout\excel\branch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\ResposAxsis\API\Service.Catalog\wwwroot\layout\excel\branch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61AA138-7733-442F-9E5D-35BE0EA3AA10}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7433C7-7493-49A3-B1EB-4B394F93486F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sucursales" sheetId="1" r:id="rId1"/>
@@ -153,10 +153,10 @@
     <t>{{Sucursales.ciudad}}</t>
   </si>
   <si>
-    <t>{{Sucursales.coloniaId}}</t>
-  </si>
-  <si>
     <t>{{Sucursales.codigoPostal}}</t>
+  </si>
+  <si>
+    <t>{{Sucursales.colonia}}</t>
   </si>
 </sst>
 </file>
@@ -611,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8A4281-45E9-4A26-88B5-8DB32AE336F4}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,7 +676,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="1" t="s">
@@ -739,7 +739,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="1" t="s">
@@ -810,13 +810,7 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E7:F7"/>
@@ -825,7 +819,13 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>